<commit_message>
atualizando status no excel quando as credenciais estiverem erradas
</commit_message>
<xml_diff>
--- a/Senha Municipio Itapira.xlsx
+++ b/Senha Municipio Itapira.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="276">
   <si>
     <t xml:space="preserve">Empresa</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t xml:space="preserve">43.248.598/0001-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">777753y</t>
   </si>
   <si>
     <t xml:space="preserve">Setembro</t>
@@ -988,31 +991,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1302,7 +1305,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1315,7 +1318,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1335,2053 +1338,2053 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="n">
-        <v>777753</v>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>667295</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>512552</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>445544</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>927104</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>271246</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>934425</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>785469</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>528965</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>437220</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F15" s="4"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F16" s="4"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>147258</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>852010</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F19" s="4"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>252622</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F20" s="4"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F21" s="4"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>394946</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>259578</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>974877</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>538014</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F27" s="4"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>935540</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F28" s="4"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>691462</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F29" s="4"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F30" s="4"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F31" s="4"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F32" s="4"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>201821</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F33" s="4"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>147258</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F34" s="4"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>562356</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F35" s="4"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F36" s="4"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>602396</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F37" s="4"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F38" s="4"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C39" s="3" t="n">
         <v>490627</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F39" s="4"/>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40" s="3" t="n">
         <v>775433</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F40" s="4"/>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C41" s="5" t="n">
         <v>118593</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F41" s="4"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F42" s="4"/>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>468106</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E43" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F43" s="4"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C44" s="3" t="n">
         <v>526958</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F44" s="4"/>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E45" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F45" s="4"/>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E46" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F46" s="4"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E47" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F47" s="4"/>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C48" s="3" t="n">
         <v>808260</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E48" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F48" s="4"/>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E49" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F49" s="4"/>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E50" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F50" s="4"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E51" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F51" s="4"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E52" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F52" s="4"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C53" s="3" t="n">
         <v>946709</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E53" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F53" s="4"/>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>185153</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E54" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F55" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E56" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F56" s="4"/>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C57" s="3" t="n">
         <v>257916</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F57" s="4"/>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>630482</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E58" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F58" s="4"/>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C59" s="3" t="n">
         <v>824790</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F59" s="4"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E60" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F61" s="4"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E63" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F63" s="4"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E64" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F64" s="4"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F65" s="4"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E66" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F66" s="4"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C67" s="3" t="n">
         <v>703851</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E67" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F67" s="4"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C68" s="3" t="n">
         <v>654456</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E68" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F68" s="4"/>
     </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E69" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F69" s="4"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F70" s="4"/>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E71" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F71" s="4"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C72" s="3" t="n">
         <v>256246</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E72" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F72" s="4"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C73" s="3" t="n">
         <v>605015</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E73" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F73" s="4"/>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C74" s="3" t="n">
         <v>494353</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E74" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F74" s="4"/>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E75" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E77" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F77" s="4"/>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C78" s="3" t="n">
         <v>166222</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C79" s="3" t="n">
         <v>801376</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E79" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F79" s="4"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C80" s="5" t="n">
         <v>830524</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E80" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E81" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F81" s="4"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C82" s="3" t="n">
         <v>575368</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E82" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F82" s="4"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E83" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F83" s="4"/>
     </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>801632</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F84" s="4"/>
     </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>526985</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E85" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F85" s="4"/>
     </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E86" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F86" s="4"/>
     </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C87" s="3" t="n">
         <v>654987</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E87" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F87" s="4"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>803716</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F88" s="4"/>
     </row>
-    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E89" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F89" s="4"/>
     </row>
-    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>725509</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F90" s="4"/>
     </row>
-    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C91" s="3" t="n">
         <v>430673</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E91" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F91" s="4"/>
     </row>
-    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>915446</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F92" s="4"/>
     </row>
-    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C93" s="3" t="n">
         <v>912955</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E93" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F93" s="4"/>
     </row>
-    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E94" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F94" s="4"/>
     </row>
-    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C95" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E95" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F95" s="4"/>
     </row>
-    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C96" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E96" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F96" s="4"/>
     </row>
-    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C97" s="3" t="n">
         <v>528965</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E97" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C98" s="3" t="n">
         <v>110346</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E98" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F98" s="4"/>
     </row>
-    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C99" s="3" t="n">
         <v>58764</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E99" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F99" s="4"/>
     </row>
-    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C100" s="3" t="n">
         <v>597014</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C101" s="3" t="n">
         <v>193303</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E101" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F101" s="4"/>
     </row>
-    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C102" s="3" t="n">
         <v>856740</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E102" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F102" s="4"/>
     </row>
-    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C103" s="3" t="n">
         <v>557082</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E103" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F103" s="4"/>
     </row>
-    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C104" s="3" t="n">
         <v>724434</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E104" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F104" s="4"/>
     </row>
-    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C105" s="3" t="n">
         <v>777111</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E105" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F105" s="4"/>
     </row>
-    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C106" s="3" t="n">
         <v>838413</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F106" s="4"/>
     </row>
-    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C107" s="3" t="n">
         <v>475916</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E107" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F107" s="4"/>
     </row>
-    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C108" s="5" t="n">
         <v>51432</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F108" s="4"/>
     </row>
-    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E109" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F109" s="4"/>
     </row>
-    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E110" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C111" s="3" t="n">
         <v>745656</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E111" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F111" s="4"/>
     </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C112" s="3" t="n">
         <v>613015</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E112" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F112" s="4"/>
     </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C113" s="3" t="n">
         <v>963963</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E113" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F113" s="4"/>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:F1">
     <sortState ref="A2:F1">
       <sortCondition ref="A2:A1" customList=""/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A106:A113 A101">
+  <conditionalFormatting sqref="A101 A106:A113">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
@@ -3399,7 +3402,7 @@
     <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:A32 A114:A1048576 A1:A26 A34:A103">
+  <conditionalFormatting sqref="A1:A26 A29:A32 A34:A103 A114:A1048576">
     <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3426,24 +3429,24 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E1" s="4" t="n">
         <v>2023</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
primeira etapa para download de boletos fiscais
</commit_message>
<xml_diff>
--- a/Senha Municipio Itapira.xlsx
+++ b/Senha Municipio Itapira.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="275">
   <si>
     <t xml:space="preserve">Empresa</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t xml:space="preserve">43.248.598/0001-45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">777753y</t>
   </si>
   <si>
     <t xml:space="preserve">Setembro</t>
@@ -991,31 +988,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1305,7 +1302,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1345,11 +1342,11 @@
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
+      <c r="C2" s="3" t="n">
+        <v>777753</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="n">
         <v>2025</v>
@@ -1358,16 +1355,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>667295</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>2025</v>
@@ -1376,16 +1373,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>2025</v>
@@ -1394,16 +1391,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
       </c>
       <c r="C5" s="3" t="n">
         <v>512552</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>2025</v>
@@ -1412,16 +1409,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>2025</v>
@@ -1430,16 +1427,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="C7" s="3" t="n">
         <v>445544</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>2025</v>
@@ -1448,16 +1445,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>2025</v>
@@ -1466,16 +1463,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C9" s="3" t="n">
         <v>927104</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>2025</v>
@@ -1484,16 +1481,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>271246</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>2025</v>
@@ -1502,16 +1499,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>934425</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>2025</v>
@@ -1520,16 +1517,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>785469</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>2025</v>
@@ -1538,16 +1535,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>34</v>
       </c>
       <c r="C13" s="3" t="n">
         <v>528965</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>2025</v>
@@ -1556,16 +1553,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="3" t="n">
         <v>437220</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>2025</v>
@@ -1574,16 +1571,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>2025</v>
@@ -1592,16 +1589,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="C16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>2025</v>
@@ -1610,16 +1607,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C17" s="5" t="n">
         <v>147258</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>2025</v>
@@ -1628,16 +1625,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="C18" s="3" t="n">
         <v>852010</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>2025</v>
@@ -1646,16 +1643,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>2025</v>
@@ -1664,16 +1661,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>252622</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>2025</v>
@@ -1682,16 +1679,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="D21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>2025</v>
@@ -1700,16 +1697,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>2025</v>
@@ -1718,16 +1715,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="D23" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>2025</v>
@@ -1736,16 +1733,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>394946</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>2025</v>
@@ -1754,16 +1751,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C25" s="3" t="n">
         <v>259578</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>2025</v>
@@ -1772,16 +1769,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>974877</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>2025</v>
@@ -1790,16 +1787,16 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>538014</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>2025</v>
@@ -1808,16 +1805,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>935540</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>2025</v>
@@ -1826,16 +1823,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>691462</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>2025</v>
@@ -1844,16 +1841,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>2025</v>
@@ -1862,16 +1859,16 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>2025</v>
@@ -1880,16 +1877,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="D32" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>2025</v>
@@ -1898,16 +1895,16 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="C33" s="3" t="n">
         <v>201821</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>2025</v>
@@ -1916,16 +1913,16 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>147258</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>2025</v>
@@ -1934,16 +1931,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>562356</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="4" t="n">
         <v>2025</v>
@@ -1952,16 +1949,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="D36" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>2025</v>
@@ -1970,16 +1967,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>90</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>602396</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>2025</v>
@@ -1988,16 +1985,16 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="D38" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E38" s="4" t="n">
         <v>2025</v>
@@ -2006,16 +2003,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>95</v>
       </c>
       <c r="C39" s="3" t="n">
         <v>490627</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>2025</v>
@@ -2024,16 +2021,16 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="C40" s="3" t="n">
         <v>775433</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>2025</v>
@@ -2042,16 +2039,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="C41" s="5" t="n">
         <v>118593</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>2025</v>
@@ -2060,16 +2057,16 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="D42" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>2025</v>
@@ -2078,16 +2075,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>468106</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" s="4" t="n">
         <v>2025</v>
@@ -2096,16 +2093,16 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B44" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>106</v>
       </c>
       <c r="C44" s="3" t="n">
         <v>526958</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>2025</v>
@@ -2114,16 +2111,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>109</v>
-      </c>
       <c r="D45" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E45" s="4" t="n">
         <v>2025</v>
@@ -2132,16 +2129,16 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="C46" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>112</v>
-      </c>
       <c r="D46" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="4" t="n">
         <v>2025</v>
@@ -2150,16 +2147,16 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C47" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="D47" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E47" s="4" t="n">
         <v>2025</v>
@@ -2168,16 +2165,16 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="C48" s="3" t="n">
         <v>808260</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" s="4" t="n">
         <v>2025</v>
@@ -2186,16 +2183,16 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>120</v>
-      </c>
       <c r="D49" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E49" s="4" t="n">
         <v>2025</v>
@@ -2204,16 +2201,16 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="D50" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E50" s="4" t="n">
         <v>2025</v>
@@ -2222,16 +2219,16 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="C51" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="D51" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E51" s="4" t="n">
         <v>2025</v>
@@ -2240,16 +2237,16 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="D52" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E52" s="4" t="n">
         <v>2025</v>
@@ -2258,16 +2255,16 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="C53" s="3" t="n">
         <v>946709</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E53" s="4" t="n">
         <v>2025</v>
@@ -2276,56 +2273,56 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>185153</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E54" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B55" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="C55" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="D55" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E55" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="D56" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E56" s="4" t="n">
         <v>2025</v>
@@ -2334,16 +2331,16 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>141</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>142</v>
       </c>
       <c r="C57" s="3" t="n">
         <v>257916</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E57" s="4" t="n">
         <v>2025</v>
@@ -2352,16 +2349,16 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>630482</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" s="4" t="n">
         <v>2025</v>
@@ -2370,16 +2367,16 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="C59" s="3" t="n">
         <v>824790</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E59" s="4" t="n">
         <v>2025</v>
@@ -2388,36 +2385,36 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="D60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F60" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="C61" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>153</v>
-      </c>
       <c r="D61" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E61" s="4" t="n">
         <v>2025</v>
@@ -2426,36 +2423,36 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="C62" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>158</v>
-      </c>
       <c r="D63" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E63" s="4" t="n">
         <v>2025</v>
@@ -2464,16 +2461,16 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B64" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="C64" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="C64" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="D64" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" s="4" t="n">
         <v>2025</v>
@@ -2482,16 +2479,16 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C65" s="3" t="s">
-        <v>164</v>
-      </c>
       <c r="D65" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E65" s="4" t="n">
         <v>2025</v>
@@ -2500,16 +2497,16 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>166</v>
-      </c>
       <c r="C66" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" s="4" t="n">
         <v>2025</v>
@@ -2518,16 +2515,16 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="C67" s="3" t="n">
         <v>703851</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E67" s="4" t="n">
         <v>2025</v>
@@ -2536,16 +2533,16 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>170</v>
       </c>
       <c r="C68" s="3" t="n">
         <v>654456</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E68" s="4" t="n">
         <v>2025</v>
@@ -2554,16 +2551,16 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="D69" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E69" s="4" t="n">
         <v>2025</v>
@@ -2572,16 +2569,16 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="C70" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="D70" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>2025</v>
@@ -2590,16 +2587,16 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="C71" s="5" t="s">
-        <v>179</v>
-      </c>
       <c r="D71" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E71" s="4" t="n">
         <v>2025</v>
@@ -2608,16 +2605,16 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B72" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="C72" s="3" t="n">
         <v>256246</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E72" s="4" t="n">
         <v>2025</v>
@@ -2626,16 +2623,16 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B73" s="3" t="s">
         <v>182</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="C73" s="3" t="n">
         <v>605015</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E73" s="4" t="n">
         <v>2025</v>
@@ -2644,16 +2641,16 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B74" s="3" t="s">
         <v>184</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>185</v>
       </c>
       <c r="C74" s="3" t="n">
         <v>494353</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E74" s="4" t="n">
         <v>2025</v>
@@ -2662,16 +2659,16 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B75" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="B75" s="3" t="s">
+      <c r="C75" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="C75" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="D75" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E75" s="4" t="n">
         <v>2025</v>
@@ -2680,16 +2677,16 @@
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C76" s="5" t="s">
-        <v>191</v>
-      </c>
       <c r="D76" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>2025</v>
@@ -2698,16 +2695,16 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B77" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="C77" s="3" t="s">
-        <v>194</v>
-      </c>
       <c r="D77" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E77" s="4" t="n">
         <v>2025</v>
@@ -2716,36 +2713,36 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B78" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="C78" s="3" t="n">
         <v>166222</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="C79" s="3" t="n">
         <v>801376</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E79" s="4" t="n">
         <v>2025</v>
@@ -2754,36 +2751,36 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="C80" s="5" t="n">
         <v>830524</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E80" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="C81" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C81" s="5" t="s">
-        <v>203</v>
-      </c>
       <c r="D81" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E81" s="4" t="n">
         <v>2025</v>
@@ -2792,16 +2789,16 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>204</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>205</v>
       </c>
       <c r="C82" s="3" t="n">
         <v>575368</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E82" s="4" t="n">
         <v>2025</v>
@@ -2810,16 +2807,16 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="C83" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>208</v>
-      </c>
       <c r="D83" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E83" s="4" t="n">
         <v>2025</v>
@@ -2828,16 +2825,16 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>209</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>210</v>
       </c>
       <c r="C84" s="3" t="n">
         <v>801632</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>2025</v>
@@ -2846,16 +2843,16 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B85" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="C85" s="3" t="n">
         <v>526985</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E85" s="4" t="n">
         <v>2025</v>
@@ -2864,16 +2861,16 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="C86" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>215</v>
-      </c>
       <c r="D86" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E86" s="4" t="n">
         <v>2025</v>
@@ -2882,16 +2879,16 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B87" s="3" t="s">
         <v>216</v>
-      </c>
-      <c r="B87" s="3" t="s">
-        <v>217</v>
       </c>
       <c r="C87" s="3" t="n">
         <v>654987</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E87" s="4" t="n">
         <v>2025</v>
@@ -2900,16 +2897,16 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>218</v>
-      </c>
-      <c r="B88" s="3" t="s">
-        <v>219</v>
       </c>
       <c r="C88" s="3" t="n">
         <v>803716</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>2025</v>
@@ -2918,16 +2915,16 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B89" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="B89" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="C89" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E89" s="4" t="n">
         <v>2025</v>
@@ -2936,16 +2933,16 @@
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B90" s="3" t="s">
         <v>222</v>
-      </c>
-      <c r="B90" s="3" t="s">
-        <v>223</v>
       </c>
       <c r="C90" s="3" t="n">
         <v>725509</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>2025</v>
@@ -2954,16 +2951,16 @@
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>224</v>
-      </c>
-      <c r="B91" s="3" t="s">
-        <v>225</v>
       </c>
       <c r="C91" s="3" t="n">
         <v>430673</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E91" s="4" t="n">
         <v>2025</v>
@@ -2972,16 +2969,16 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B92" s="3" t="s">
         <v>226</v>
-      </c>
-      <c r="B92" s="3" t="s">
-        <v>227</v>
       </c>
       <c r="C92" s="3" t="n">
         <v>915446</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>2025</v>
@@ -2990,16 +2987,16 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="C93" s="3" t="n">
         <v>912955</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E93" s="4" t="n">
         <v>2025</v>
@@ -3008,16 +3005,16 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B94" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="C94" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="C94" s="5" t="s">
-        <v>232</v>
-      </c>
       <c r="D94" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E94" s="4" t="n">
         <v>2025</v>
@@ -3026,16 +3023,16 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B95" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B95" s="6" t="s">
-        <v>234</v>
-      </c>
       <c r="C95" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E95" s="4" t="n">
         <v>2025</v>
@@ -3044,16 +3041,16 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B96" s="3" t="s">
         <v>235</v>
-      </c>
-      <c r="B96" s="3" t="s">
-        <v>236</v>
       </c>
       <c r="C96" s="3" t="n">
         <v>123456</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E96" s="4" t="n">
         <v>2025</v>
@@ -3062,36 +3059,36 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B97" s="3" t="s">
         <v>237</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>238</v>
       </c>
       <c r="C97" s="3" t="n">
         <v>528965</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E97" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>241</v>
       </c>
       <c r="C98" s="3" t="n">
         <v>110346</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E98" s="4" t="n">
         <v>2025</v>
@@ -3100,16 +3097,16 @@
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>242</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>243</v>
       </c>
       <c r="C99" s="3" t="n">
         <v>58764</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E99" s="4" t="n">
         <v>2025</v>
@@ -3118,36 +3115,36 @@
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B100" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>245</v>
       </c>
       <c r="C100" s="3" t="n">
         <v>597014</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B101" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="B101" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="C101" s="3" t="n">
         <v>193303</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E101" s="4" t="n">
         <v>2025</v>
@@ -3156,16 +3153,16 @@
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>248</v>
-      </c>
-      <c r="B102" s="3" t="s">
-        <v>249</v>
       </c>
       <c r="C102" s="3" t="n">
         <v>856740</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E102" s="4" t="n">
         <v>2025</v>
@@ -3174,16 +3171,16 @@
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B103" s="3" t="s">
         <v>250</v>
-      </c>
-      <c r="B103" s="3" t="s">
-        <v>251</v>
       </c>
       <c r="C103" s="3" t="n">
         <v>557082</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E103" s="4" t="n">
         <v>2025</v>
@@ -3192,16 +3189,16 @@
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="B104" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="C104" s="3" t="n">
         <v>724434</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E104" s="4" t="n">
         <v>2025</v>
@@ -3210,16 +3207,16 @@
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B105" s="3" t="s">
         <v>254</v>
-      </c>
-      <c r="B105" s="3" t="s">
-        <v>255</v>
       </c>
       <c r="C105" s="3" t="n">
         <v>777111</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E105" s="4" t="n">
         <v>2025</v>
@@ -3228,16 +3225,16 @@
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="B106" s="3" t="s">
-        <v>257</v>
       </c>
       <c r="C106" s="3" t="n">
         <v>838413</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>2025</v>
@@ -3246,16 +3243,16 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>258</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>259</v>
       </c>
       <c r="C107" s="3" t="n">
         <v>475916</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E107" s="4" t="n">
         <v>2025</v>
@@ -3264,16 +3261,16 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>260</v>
-      </c>
-      <c r="B108" s="3" t="s">
-        <v>261</v>
       </c>
       <c r="C108" s="5" t="n">
         <v>51432</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>2025</v>
@@ -3282,16 +3279,16 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B109" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="C109" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="C109" s="5" t="s">
-        <v>264</v>
-      </c>
       <c r="D109" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E109" s="4" t="n">
         <v>2025</v>
@@ -3300,16 +3297,16 @@
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B110" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="C110" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E110" s="4" t="n">
         <v>2025</v>
@@ -3318,16 +3315,16 @@
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="C111" s="3" t="n">
         <v>745656</v>
       </c>
       <c r="D111" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E111" s="4" t="n">
         <v>2025</v>
@@ -3336,16 +3333,16 @@
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B112" s="3" t="s">
         <v>269</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>270</v>
       </c>
       <c r="C112" s="3" t="n">
         <v>613015</v>
       </c>
       <c r="D112" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E112" s="4" t="n">
         <v>2025</v>
@@ -3354,16 +3351,16 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B113" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="C113" s="3" t="n">
         <v>963963</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E113" s="4" t="n">
         <v>2025</v>
@@ -3431,22 +3428,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>275</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="4" t="n">
         <v>2023</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ajustado log caso o alerta de finalizaçao de escrituração nao apareça
</commit_message>
<xml_diff>
--- a/Senha Municipio Itapira.xlsx
+++ b/Senha Municipio Itapira.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="269">
   <si>
     <t xml:space="preserve">Empresa</t>
   </si>
@@ -44,43 +44,25 @@
     <t xml:space="preserve">Status Processo</t>
   </si>
   <si>
-    <t xml:space="preserve">ATILIO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.248.598/0001-45</t>
+    <t xml:space="preserve">BAZAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49.918.766/0001-49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Outubro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDBUENO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.750.720/0001-87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">760915</t>
   </si>
   <si>
     <t xml:space="preserve">Setembro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATIVA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02.867.598/0001-46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AUDIUM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03.978.105/0001-08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">451417</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAZAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49.918.766/0001-49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BDBUENO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43.750.720/0001-87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">760915</t>
   </si>
   <si>
     <t xml:space="preserve">BEACH</t>
@@ -1302,7 +1284,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1343,7 +1325,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>777753</v>
+        <v>512552</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -1360,11 +1342,11 @@
       <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="n">
-        <v>667295</v>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="n">
         <v>2025</v>
@@ -1373,16 +1355,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>445544</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="n">
         <v>2025</v>
@@ -1391,16 +1373,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>512552</v>
+      <c r="B5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E5" s="4" t="n">
         <v>2025</v>
@@ -1409,16 +1391,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>927104</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E6" s="4" t="n">
         <v>2025</v>
@@ -1427,16 +1409,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>445544</v>
+        <v>271246</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E7" s="4" t="n">
         <v>2025</v>
@@ -1445,16 +1427,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="C8" s="3" t="n">
+        <v>934425</v>
+      </c>
       <c r="D8" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E8" s="4" t="n">
         <v>2025</v>
@@ -1469,10 +1451,10 @@
         <v>25</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>927104</v>
+        <v>785469</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E9" s="4" t="n">
         <v>2025</v>
@@ -1487,10 +1469,10 @@
         <v>27</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>271246</v>
+        <v>528965</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E10" s="4" t="n">
         <v>2025</v>
@@ -1505,10 +1487,10 @@
         <v>29</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>934425</v>
+        <v>437220</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E11" s="4" t="n">
         <v>2025</v>
@@ -1523,10 +1505,10 @@
         <v>31</v>
       </c>
       <c r="C12" s="3" t="n">
-        <v>785469</v>
+        <v>123456</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E12" s="4" t="n">
         <v>2025</v>
@@ -1537,14 +1519,14 @@
       <c r="A13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="n">
-        <v>528965</v>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E13" s="4" t="n">
         <v>2025</v>
@@ -1553,16 +1535,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>437220</v>
+        <v>36</v>
+      </c>
+      <c r="C14" s="5" t="n">
+        <v>147258</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E14" s="4" t="n">
         <v>2025</v>
@@ -1571,16 +1553,16 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="3" t="n">
-        <v>123456</v>
+        <v>852010</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E15" s="4" t="n">
         <v>2025</v>
@@ -1589,16 +1571,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>40</v>
       </c>
+      <c r="C16" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D16" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E16" s="4" t="n">
         <v>2025</v>
@@ -1607,16 +1589,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="5" t="n">
-        <v>147258</v>
+        <v>43</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>252622</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E17" s="4" t="n">
         <v>2025</v>
@@ -1625,16 +1607,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="3" t="n">
-        <v>852010</v>
+      <c r="B18" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E18" s="4" t="n">
         <v>2025</v>
@@ -1643,16 +1625,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E19" s="4" t="n">
         <v>2025</v>
@@ -1661,16 +1643,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>252622</v>
+        <v>50</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E20" s="4" t="n">
         <v>2025</v>
@@ -1679,16 +1661,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>394946</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E21" s="4" t="n">
         <v>2025</v>
@@ -1697,16 +1679,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>259578</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E22" s="4" t="n">
         <v>2025</v>
@@ -1715,16 +1697,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="C23" s="3" t="n">
+        <v>974877</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E23" s="4" t="n">
         <v>2025</v>
@@ -1739,10 +1721,10 @@
         <v>60</v>
       </c>
       <c r="C24" s="3" t="n">
-        <v>394946</v>
+        <v>538014</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E24" s="4" t="n">
         <v>2025</v>
@@ -1757,10 +1739,10 @@
         <v>62</v>
       </c>
       <c r="C25" s="3" t="n">
-        <v>259578</v>
+        <v>935540</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E25" s="4" t="n">
         <v>2025</v>
@@ -1775,10 +1757,10 @@
         <v>64</v>
       </c>
       <c r="C26" s="3" t="n">
-        <v>974877</v>
+        <v>691462</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E26" s="4" t="n">
         <v>2025</v>
@@ -1789,14 +1771,14 @@
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="3" t="n">
-        <v>538014</v>
+      <c r="C27" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E27" s="4" t="n">
         <v>2025</v>
@@ -1805,16 +1787,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28" s="3" t="n">
-        <v>935540</v>
+        <v>123456</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E28" s="4" t="n">
         <v>2025</v>
@@ -1823,16 +1805,16 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="3" t="n">
-        <v>691462</v>
+      <c r="B29" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E29" s="4" t="n">
         <v>2025</v>
@@ -1841,16 +1823,16 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" s="5" t="s">
         <v>73</v>
       </c>
+      <c r="B30" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>201821</v>
+      </c>
       <c r="D30" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E30" s="4" t="n">
         <v>2025</v>
@@ -1859,16 +1841,16 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C31" s="3" t="n">
-        <v>123456</v>
+        <v>147258</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E31" s="4" t="n">
         <v>2025</v>
@@ -1877,16 +1859,16 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B32" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="C32" s="3" t="n">
+        <v>562356</v>
+      </c>
       <c r="D32" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E32" s="4" t="n">
         <v>2025</v>
@@ -1900,11 +1882,11 @@
       <c r="B33" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="3" t="n">
-        <v>201821</v>
+      <c r="C33" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E33" s="4" t="n">
         <v>2025</v>
@@ -1913,16 +1895,16 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34" s="3" t="n">
-        <v>147258</v>
+        <v>602396</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E34" s="4" t="n">
         <v>2025</v>
@@ -1931,16 +1913,16 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C35" s="3" t="n">
-        <v>562356</v>
+      <c r="B35" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E35" s="4" t="n">
         <v>2025</v>
@@ -1949,16 +1931,16 @@
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>490627</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E36" s="4" t="n">
         <v>2025</v>
@@ -1967,16 +1949,16 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C37" s="3" t="n">
-        <v>602396</v>
+        <v>775433</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E37" s="4" t="n">
         <v>2025</v>
@@ -1985,16 +1967,16 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="B38" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="C38" s="5" t="n">
+        <v>118593</v>
+      </c>
       <c r="D38" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E38" s="4" t="n">
         <v>2025</v>
@@ -2008,11 +1990,11 @@
       <c r="B39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="3" t="n">
-        <v>490627</v>
+      <c r="C39" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E39" s="4" t="n">
         <v>2025</v>
@@ -2021,16 +2003,16 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40" s="3" t="n">
-        <v>775433</v>
+        <v>468106</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E40" s="4" t="n">
         <v>2025</v>
@@ -2039,16 +2021,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C41" s="5" t="n">
-        <v>118593</v>
+        <v>99</v>
+      </c>
+      <c r="C41" s="3" t="n">
+        <v>526958</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E41" s="4" t="n">
         <v>2025</v>
@@ -2057,16 +2039,16 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E42" s="4" t="n">
         <v>2025</v>
@@ -2075,16 +2057,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="3" t="n">
-        <v>468106</v>
+        <v>104</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E43" s="4" t="n">
         <v>2025</v>
@@ -2093,16 +2075,16 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="3" t="n">
-        <v>526958</v>
+        <v>106</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E44" s="4" t="n">
         <v>2025</v>
@@ -2111,16 +2093,16 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="C45" s="3" t="n">
+        <v>808260</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E45" s="4" t="n">
         <v>2025</v>
@@ -2129,16 +2111,16 @@
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E46" s="4" t="n">
         <v>2025</v>
@@ -2147,16 +2129,16 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C47" s="5" t="s">
         <v>114</v>
       </c>
+      <c r="B47" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="D47" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E47" s="4" t="n">
         <v>2025</v>
@@ -2165,16 +2147,16 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C48" s="3" t="n">
-        <v>808260</v>
+        <v>118</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E48" s="4" t="n">
         <v>2025</v>
@@ -2183,16 +2165,16 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E49" s="4" t="n">
         <v>2025</v>
@@ -2201,16 +2183,16 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
+      </c>
+      <c r="C50" s="3" t="n">
+        <v>946709</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E50" s="4" t="n">
         <v>2025</v>
@@ -2219,52 +2201,56 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
+      </c>
+      <c r="C51" s="3" t="n">
+        <v>185153</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E51" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F51" s="4"/>
+      <c r="F51" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B52" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" s="4" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F52" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C53" s="3" t="n">
-        <v>946709</v>
+        <v>132</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E53" s="4" t="n">
         <v>2025</v>
@@ -2273,56 +2259,52 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C54" s="3" t="n">
-        <v>185153</v>
+        <v>257916</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E54" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F54" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="F54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C55" s="5" t="s">
         <v>136</v>
       </c>
+      <c r="B55" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="3" t="n">
+        <v>630482</v>
+      </c>
       <c r="D55" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E55" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="F55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C56" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="C56" s="3" t="n">
+        <v>824790</v>
+      </c>
       <c r="D56" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E56" s="4" t="n">
         <v>2025</v>
@@ -2336,29 +2318,31 @@
       <c r="B57" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C57" s="3" t="n">
-        <v>257916</v>
+      <c r="C57" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E57" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F57" s="4"/>
+      <c r="F57" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C58" s="3" t="n">
-        <v>630482</v>
+        <v>144</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>146</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E58" s="4" t="n">
         <v>2025</v>
@@ -2367,54 +2351,54 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C59" s="3" t="n">
-        <v>824790</v>
+        <v>148</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E59" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F59" s="4"/>
+      <c r="F59" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E60" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="F60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="C61" s="5" t="s">
         <v>152</v>
       </c>
+      <c r="B61" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="D61" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E61" s="4" t="n">
         <v>2025</v>
@@ -2423,36 +2407,34 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E62" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="F62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>157</v>
+        <v>52</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E63" s="4" t="n">
         <v>2025</v>
@@ -2461,16 +2443,16 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C64" s="6" t="s">
         <v>160</v>
       </c>
+      <c r="B64" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="3" t="n">
+        <v>703851</v>
+      </c>
       <c r="D64" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E64" s="4" t="n">
         <v>2025</v>
@@ -2479,16 +2461,16 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C65" s="3" t="s">
         <v>163</v>
       </c>
+      <c r="C65" s="3" t="n">
+        <v>654456</v>
+      </c>
       <c r="D65" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E65" s="4" t="n">
         <v>2025</v>
@@ -2499,14 +2481,14 @@
       <c r="A66" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C66" s="5" t="s">
-        <v>58</v>
+      <c r="C66" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E66" s="4" t="n">
         <v>2025</v>
@@ -2515,16 +2497,16 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C67" s="3" t="n">
-        <v>703851</v>
+        <v>168</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>169</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E67" s="4" t="n">
         <v>2025</v>
@@ -2533,16 +2515,16 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="C68" s="3" t="n">
-        <v>654456</v>
+        <v>170</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E68" s="4" t="n">
         <v>2025</v>
@@ -2551,16 +2533,16 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+      <c r="C69" s="3" t="n">
+        <v>256246</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E69" s="4" t="n">
         <v>2025</v>
@@ -2569,16 +2551,16 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="C70" s="3" t="n">
+        <v>605015</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E70" s="4" t="n">
         <v>2025</v>
@@ -2587,16 +2569,16 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B71" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="B71" s="3" t="s">
         <v>178</v>
       </c>
+      <c r="C71" s="3" t="n">
+        <v>494353</v>
+      </c>
       <c r="D71" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E71" s="4" t="n">
         <v>2025</v>
@@ -2610,11 +2592,11 @@
       <c r="B72" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C72" s="3" t="n">
-        <v>256246</v>
+      <c r="C72" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E72" s="4" t="n">
         <v>2025</v>
@@ -2623,16 +2605,16 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C73" s="3" t="n">
-        <v>605015</v>
+        <v>183</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E73" s="4" t="n">
         <v>2025</v>
@@ -2641,16 +2623,16 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C74" s="3" t="n">
-        <v>494353</v>
+        <v>186</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>187</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E74" s="4" t="n">
         <v>2025</v>
@@ -2659,34 +2641,36 @@
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
+      </c>
+      <c r="C75" s="3" t="n">
+        <v>166222</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E75" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F75" s="4"/>
+      <c r="F75" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C76" s="5" t="s">
-        <v>190</v>
+        <v>191</v>
+      </c>
+      <c r="C76" s="3" t="n">
+        <v>801376</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E76" s="4" t="n">
         <v>2025</v>
@@ -2695,54 +2679,54 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="C77" s="3" t="s">
         <v>193</v>
       </c>
+      <c r="C77" s="5" t="n">
+        <v>830524</v>
+      </c>
       <c r="D77" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E77" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F77" s="4"/>
+      <c r="F77" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="C78" s="3" t="n">
-        <v>166222</v>
+      <c r="C78" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E78" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="F78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C79" s="3" t="n">
-        <v>801376</v>
+        <v>575368</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E79" s="4" t="n">
         <v>2025</v>
@@ -2751,36 +2735,34 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B80" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="C80" s="5" t="n">
-        <v>830524</v>
+      <c r="B80" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E80" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F80" s="4" t="s">
-        <v>149</v>
-      </c>
+      <c r="F80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="C81" s="5" t="s">
         <v>202</v>
       </c>
+      <c r="B81" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C81" s="3" t="n">
+        <v>801632</v>
+      </c>
       <c r="D81" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E81" s="4" t="n">
         <v>2025</v>
@@ -2789,16 +2771,16 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C82" s="3" t="n">
-        <v>575368</v>
+        <v>526985</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E82" s="4" t="n">
         <v>2025</v>
@@ -2807,16 +2789,16 @@
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="C83" s="3" t="s">
         <v>207</v>
       </c>
+      <c r="C83" s="5" t="s">
+        <v>208</v>
+      </c>
       <c r="D83" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E83" s="4" t="n">
         <v>2025</v>
@@ -2825,16 +2807,16 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C84" s="3" t="n">
-        <v>801632</v>
+        <v>654987</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E84" s="4" t="n">
         <v>2025</v>
@@ -2843,16 +2825,16 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C85" s="3" t="n">
-        <v>526985</v>
+        <v>803716</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E85" s="4" t="n">
         <v>2025</v>
@@ -2861,16 +2843,16 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="B86" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C86" s="5" t="s">
+      <c r="B86" s="3" t="s">
         <v>214</v>
       </c>
+      <c r="C86" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="D86" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E86" s="4" t="n">
         <v>2025</v>
@@ -2885,10 +2867,10 @@
         <v>216</v>
       </c>
       <c r="C87" s="3" t="n">
-        <v>654987</v>
+        <v>725509</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E87" s="4" t="n">
         <v>2025</v>
@@ -2903,10 +2885,10 @@
         <v>218</v>
       </c>
       <c r="C88" s="3" t="n">
-        <v>803716</v>
+        <v>430673</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E88" s="4" t="n">
         <v>2025</v>
@@ -2920,11 +2902,11 @@
       <c r="B89" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>23</v>
+      <c r="C89" s="3" t="n">
+        <v>915446</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E89" s="4" t="n">
         <v>2025</v>
@@ -2939,10 +2921,10 @@
         <v>222</v>
       </c>
       <c r="C90" s="3" t="n">
-        <v>725509</v>
+        <v>912955</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E90" s="4" t="n">
         <v>2025</v>
@@ -2953,14 +2935,14 @@
       <c r="A91" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C91" s="3" t="n">
-        <v>430673</v>
+      <c r="C91" s="5" t="s">
+        <v>225</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E91" s="4" t="n">
         <v>2025</v>
@@ -2969,16 +2951,16 @@
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B92" s="3" t="s">
         <v>226</v>
       </c>
-      <c r="C92" s="3" t="n">
-        <v>915446</v>
+      <c r="B92" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E92" s="4" t="n">
         <v>2025</v>
@@ -2987,16 +2969,16 @@
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C93" s="3" t="n">
-        <v>912955</v>
+        <v>123456</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E93" s="4" t="n">
         <v>2025</v>
@@ -3005,34 +2987,36 @@
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="B94" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="B94" s="3" t="s">
         <v>231</v>
       </c>
+      <c r="C94" s="3" t="n">
+        <v>528965</v>
+      </c>
       <c r="D94" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E94" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F94" s="4"/>
+      <c r="F94" s="4" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B95" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>58</v>
+      <c r="B95" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C95" s="3" t="n">
+        <v>110346</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E95" s="4" t="n">
         <v>2025</v>
@@ -3041,16 +3025,16 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C96" s="3" t="n">
-        <v>123456</v>
+        <v>58764</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E96" s="4" t="n">
         <v>2025</v>
@@ -3059,22 +3043,22 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C97" s="3" t="n">
-        <v>528965</v>
+        <v>597014</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E97" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F97" s="4" t="s">
-        <v>238</v>
+        <v>127</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3085,10 +3069,10 @@
         <v>240</v>
       </c>
       <c r="C98" s="3" t="n">
-        <v>110346</v>
+        <v>193303</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E98" s="4" t="n">
         <v>2025</v>
@@ -3103,10 +3087,10 @@
         <v>242</v>
       </c>
       <c r="C99" s="3" t="n">
-        <v>58764</v>
+        <v>856740</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E99" s="4" t="n">
         <v>2025</v>
@@ -3121,17 +3105,15 @@
         <v>244</v>
       </c>
       <c r="C100" s="3" t="n">
-        <v>597014</v>
+        <v>557082</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E100" s="4" t="n">
         <v>2025</v>
       </c>
-      <c r="F100" s="4" t="s">
-        <v>133</v>
-      </c>
+      <c r="F100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
@@ -3141,10 +3123,10 @@
         <v>246</v>
       </c>
       <c r="C101" s="3" t="n">
-        <v>193303</v>
+        <v>724434</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E101" s="4" t="n">
         <v>2025</v>
@@ -3159,10 +3141,10 @@
         <v>248</v>
       </c>
       <c r="C102" s="3" t="n">
-        <v>856740</v>
+        <v>777111</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E102" s="4" t="n">
         <v>2025</v>
@@ -3177,10 +3159,10 @@
         <v>250</v>
       </c>
       <c r="C103" s="3" t="n">
-        <v>557082</v>
+        <v>838413</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E103" s="4" t="n">
         <v>2025</v>
@@ -3195,10 +3177,10 @@
         <v>252</v>
       </c>
       <c r="C104" s="3" t="n">
-        <v>724434</v>
+        <v>475916</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E104" s="4" t="n">
         <v>2025</v>
@@ -3212,11 +3194,11 @@
       <c r="B105" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C105" s="3" t="n">
-        <v>777111</v>
+      <c r="C105" s="5" t="n">
+        <v>51432</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E105" s="4" t="n">
         <v>2025</v>
@@ -3227,14 +3209,14 @@
       <c r="A106" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C106" s="3" t="n">
-        <v>838413</v>
+      <c r="C106" s="5" t="s">
+        <v>257</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E106" s="4" t="n">
         <v>2025</v>
@@ -3243,16 +3225,16 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B107" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="C107" s="3" t="n">
-        <v>475916</v>
+      <c r="B107" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E107" s="4" t="n">
         <v>2025</v>
@@ -3261,16 +3243,16 @@
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C108" s="5" t="n">
-        <v>51432</v>
+        <v>261</v>
+      </c>
+      <c r="C108" s="3" t="n">
+        <v>745656</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E108" s="4" t="n">
         <v>2025</v>
@@ -3279,16 +3261,16 @@
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="B109" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C109" s="5" t="s">
+      <c r="B109" s="3" t="s">
         <v>263</v>
       </c>
+      <c r="C109" s="3" t="n">
+        <v>613015</v>
+      </c>
       <c r="D109" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E109" s="4" t="n">
         <v>2025</v>
@@ -3299,94 +3281,43 @@
       <c r="A110" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C110" s="5" t="s">
-        <v>58</v>
+      <c r="C110" s="3" t="n">
+        <v>963963</v>
       </c>
       <c r="D110" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E110" s="4" t="n">
         <v>2025</v>
       </c>
       <c r="F110" s="4"/>
     </row>
-    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C111" s="3" t="n">
-        <v>745656</v>
-      </c>
-      <c r="D111" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E111" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F111" s="4"/>
-    </row>
-    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C112" s="3" t="n">
-        <v>613015</v>
-      </c>
-      <c r="D112" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E112" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F112" s="4"/>
-    </row>
-    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="B113" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C113" s="3" t="n">
-        <v>963963</v>
-      </c>
-      <c r="D113" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E113" s="4" t="n">
-        <v>2025</v>
-      </c>
-      <c r="F113" s="4"/>
-    </row>
+    <row r="1048566" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048569" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048570" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:F1">
     <sortState ref="A2:F1">
       <sortCondition ref="A2:A1" customList=""/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A101 A106:A113">
+  <conditionalFormatting sqref="A98 A103:A110">
     <cfRule type="duplicateValues" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33 A104:A105">
+  <conditionalFormatting sqref="A30 A101:A102">
     <cfRule type="duplicateValues" priority="5" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
@@ -3395,11 +3326,11 @@
     <cfRule type="duplicateValues" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A27:A28">
+  <conditionalFormatting sqref="A24:A25">
     <cfRule type="duplicateValues" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
     <cfRule type="duplicateValues" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A26 A29:A32 A34:A103 A114:A1048576">
+  <conditionalFormatting sqref="A1:A23 A26:A29 A31:A100 A111:A1048576">
     <cfRule type="duplicateValues" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2"/>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3428,22 +3359,22 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E1" s="4" t="n">
         <v>2023</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>